<commit_message>
fixed pam data which caused error in generating events
</commit_message>
<xml_diff>
--- a/src/data/bankA/PAM_Portfolio.xlsx
+++ b/src/data/bankA/PAM_Portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viganhamzai/Documents/ZHAW_WI/07_Semester/PA/PA_FEMS/src/data/bankA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E3EA38-D8BF-754D-83A2-DF1A405445F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF970ABA-C790-784E-883A-3763F40B760F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EB6AEAA4-A44D-D74E-B6F0-4D027B99E743}"/>
   </bookViews>
@@ -323,11 +323,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,7 +643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA33D00-6807-F443-9469-E95E09AFC35B}">
   <dimension ref="A1:BH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -978,7 +979,7 @@
       <c r="AA2">
         <v>0</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AB2" s="1">
         <f>DATE(YEAR(Z2)+10,MONTH(Z2),DAY(Z2))</f>
         <v>48214</v>
       </c>
@@ -1164,7 +1165,7 @@
       <c r="AA3">
         <v>0</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AB3" s="1">
         <f>DATE(YEAR(Z3)+10,MONTH(Z3),DAY(Z3))</f>
         <v>48214</v>
       </c>
@@ -1350,7 +1351,7 @@
       <c r="AA4">
         <v>0</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AB4" s="1">
         <f>DATE(YEAR(Z4)+10,MONTH(Z4),DAY(Z4))</f>
         <v>48214</v>
       </c>
@@ -1537,7 +1538,7 @@
       <c r="AA5">
         <v>0</v>
       </c>
-      <c r="AB5" s="3">
+      <c r="AB5" s="1">
         <f>DATE(YEAR(Z5)+10,MONTH(Z5),DAY(Z5))</f>
         <v>48214</v>
       </c>

</xml_diff>